<commit_message>
update: readme & manual
</commit_message>
<xml_diff>
--- a/docs/examples/nodelist.xlsx
+++ b/docs/examples/nodelist.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20352"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProgramData\kasini3000\docs\examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user001\Documents\kasini3000\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A71331E7-54D4-44DB-AD67-E3B33BB4BC4B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8658E48-DFE5-4827-A806-47B925CF2D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10335" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1815" yWindow="1815" windowWidth="21600" windowHeight="10920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nodelist" sheetId="1" r:id="rId1"/>
+    <sheet name="group_var" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="68">
   <si>
     <t>ip</t>
   </si>
@@ -73,10 +74,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>srv2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>bbbb</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -201,18 +198,10 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>uuid</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>中文字段名：</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>被控机uuid</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>端口</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -258,6 +247,46 @@
   </si>
   <si>
     <t>user2oldpwd</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>服务器2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>组2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>组1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>变量名2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>变量名3</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>变量名4</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>aaa</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bbb</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>中日韩文变量名1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>中日韩文变量值1</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1263,10 +1292,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1283,32 +1312,31 @@
     <col min="11" max="11" width="16.375" customWidth="1"/>
     <col min="12" max="13" width="27.625" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="17.25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="22.5" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G2" s="7" t="s">
         <v>3</v>
@@ -1317,31 +1345,28 @@
         <v>4</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>13</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="O2" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="17.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:15" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1357,7 +1382,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -1367,25 +1392,24 @@
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-    </row>
-    <row r="4" spans="1:16" ht="17.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:15" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -1395,26 +1419,25 @@
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-    </row>
-    <row r="5" spans="1:16" s="5" customFormat="1" ht="69" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:15" s="5" customFormat="1" ht="69" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="C5" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>10</v>
@@ -1429,27 +1452,24 @@
         <v>10</v>
       </c>
       <c r="N5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="O5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="51.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:15" ht="51.75" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -1459,14 +1479,13 @@
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="P6" s="3"/>
-    </row>
-    <row r="7" spans="1:16" ht="17.25" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -1475,7 +1494,7 @@
         <v>6</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -1485,14 +1504,13 @@
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="P7" s="3"/>
-    </row>
-    <row r="8" spans="1:16" ht="17.25" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1509,20 +1527,19 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="P8" s="3"/>
-    </row>
-    <row r="9" spans="1:16" ht="17.25" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -1534,17 +1551,16 @@
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="P9" s="3"/>
-    </row>
-    <row r="10" spans="1:16" ht="17.25" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -1556,15 +1572,14 @@
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-    </row>
-    <row r="11" spans="1:16" ht="17.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:15" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -1576,15 +1591,14 @@
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-    </row>
-    <row r="12" spans="1:16" ht="17.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:15" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
@@ -1596,11 +1610,10 @@
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-    </row>
-    <row r="13" spans="1:16" ht="17.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:15" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1616,53 +1629,49 @@
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-    </row>
-    <row r="14" spans="1:16" ht="22.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:15" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D14" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="F14" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="H14" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="G14" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>59</v>
-      </c>
       <c r="I14" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="K14" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="K14" s="8" t="s">
-        <v>60</v>
       </c>
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
       <c r="N14" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="O14" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="O14" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="P14" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="17.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:15" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1678,9 +1687,8 @@
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-    </row>
-    <row r="16" spans="1:16" ht="17.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:15" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1696,9 +1704,8 @@
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-    </row>
-    <row r="17" spans="1:16" ht="17.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:15" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1714,9 +1721,8 @@
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-    </row>
-    <row r="18" spans="1:16" ht="17.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:15" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1732,9 +1738,8 @@
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
-    </row>
-    <row r="19" spans="1:16" ht="17.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:15" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1750,9 +1755,8 @@
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-    </row>
-    <row r="20" spans="1:16" ht="17.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:15" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1768,12 +1772,11 @@
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-    </row>
-    <row r="22" spans="1:16" ht="17.25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:15" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
     </row>
-    <row r="25" spans="1:16" ht="17.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" ht="17.25" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
     </row>
   </sheetData>
@@ -1781,4 +1784,64 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69028F32-F191-48C0-8102-E5F6C7E95010}">
+  <dimension ref="A2:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.375" customWidth="1"/>
+    <col min="2" max="2" width="25.125" customWidth="1"/>
+    <col min="3" max="3" width="13.25" customWidth="1"/>
+    <col min="4" max="4" width="12.375" customWidth="1"/>
+    <col min="5" max="5" width="13.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
 </file>
</xml_diff>